<commit_message>
added JS to ipynb to hide/show input code
</commit_message>
<xml_diff>
--- a/VWSabbreviations.xlsx
+++ b/VWSabbreviations.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{054990EB-9FB9-4440-8B71-70D96E2C8D85}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView activeTab="0" windowHeight="7980" windowWidth="21570" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="List" sheetId="1" r:id="rId1"/>
@@ -416,56 +416,126 @@
   <si>
     <t>Prefix for opposing wrestler</t>
   </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>GB</t>
+  </si>
+  <si>
+    <t>Exposire</t>
+  </si>
+  <si>
+    <t>Exposure</t>
+  </si>
+  <si>
+    <t>Recovery</t>
+  </si>
+  <si>
+    <t>Gut</t>
+  </si>
+  <si>
+    <t>LegLace</t>
+  </si>
+  <si>
+    <t>Turn</t>
+  </si>
+  <si>
+    <t>Passive</t>
+  </si>
+  <si>
+    <t>Technical</t>
+  </si>
+  <si>
+    <t>Pushout</t>
+  </si>
+  <si>
+    <t>Expo</t>
+  </si>
+  <si>
+    <t>Passivity of one wrestler</t>
+  </si>
+  <si>
+    <t>Neutral technique for forcing another wrestler to expose their back</t>
+  </si>
+  <si>
+    <t>Recovering action after being exposed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Top technique </t>
+  </si>
+  <si>
+    <t>Top technique focuses on legs</t>
+  </si>
+  <si>
+    <t>Top technique focuses on torso</t>
+  </si>
+  <si>
+    <t>Alternative top techniques</t>
+  </si>
+  <si>
+    <t>Weight for compeition in kilograms</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <numFmts count="8">
+    <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);(&quot;$&quot;#,##0)"/>
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red](&quot;$&quot;#,##0)"/>
+    <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00_);(&quot;$&quot;#,##0.00)"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red](&quot;$&quot;#,##0.00)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* (#,##0);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* (#,##0);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* (#,##0.00);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* (#,##0.00);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="6">
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1" tint="0.34998626667073579"/>
       <name val="Arial"/>
       <family val="2"/>
+      <b/>
+      <color rgb="FF595959"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="4"/>
       <name val="Arial"/>
       <family val="2"/>
+      <b/>
+      <color rgb="FF1C639E"/>
+      <sz val="13"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="19"/>
-      <color theme="1" tint="0.14996795556505021"/>
       <name val="Arial"/>
       <family val="2"/>
+      <b/>
+      <color rgb="FF262626"/>
+      <sz val="19"/>
       <scheme val="major"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="4"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF1C639E"/>
+      <sz val="10"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1" tint="0.14990691854609822"/>
       <name val="Arial"/>
       <family val="2"/>
+      <b/>
+      <color rgb="FF262626"/>
+      <sz val="11"/>
       <scheme val="major"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1" tint="0.34998626667073579"/>
       <name val="Arial"/>
       <family val="2"/>
+      <color rgb="FF595959"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -479,55 +549,65 @@
   </fills>
   <borders count="1">
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
+      <left style="none">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="none">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="none">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="none">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal style="none">
+        <color rgb="FF000000"/>
+      </diagonal>
     </border>
   </borders>
   <cellStyleXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="5">
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="5" applyFill="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Date" xfId="5" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Date" xfId="5"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
@@ -886,18 +966,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView showGridLines="0" workbookViewId="0" tabSelected="1" zoomScaleNormal="100">
+      <selection pane="topLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="30"/>
   <cols>
     <col min="1" max="1" width="2.625" customWidth="1"/>
     <col min="2" max="2" width="29.75" bestFit="1" customWidth="1"/>
@@ -906,18 +985,18 @@
     <col min="5" max="5" width="17.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row ht="26.25" customHeight="1" r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="5"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="24" x14ac:dyDescent="0.25">
+    <row ht="24" r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row ht="22.15" customHeight="1" r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
@@ -931,12 +1010,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row ht="22.15" customHeight="1" r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>124</v>
+      <c r="C4" s="0" t="s">
+        <v>129</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>127</v>
@@ -945,7 +1024,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="22.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row ht="22.15" customHeight="1" r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
         <v>125</v>
       </c>
@@ -959,21 +1038,21 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row ht="30" customHeight="1" r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
         <v>67</v>
       </c>
       <c r="C6" t="s">
         <v>68</v>
       </c>
-      <c r="D6" t="s">
-        <v>71</v>
+      <c r="D6" s="0" t="s">
+        <v>148</v>
       </c>
       <c r="E6" s="7" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row ht="30" customHeight="1" r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
         <v>119</v>
       </c>
@@ -987,7 +1066,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row ht="30" customHeight="1" r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
         <v>105</v>
       </c>
@@ -1001,7 +1080,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row ht="30" customHeight="1" r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
         <v>114</v>
       </c>
@@ -1015,7 +1094,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row ht="30" customHeight="1" r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
         <v>115</v>
       </c>
@@ -1029,7 +1108,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row ht="30" customHeight="1" r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
         <v>39</v>
       </c>
@@ -1043,7 +1122,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row ht="30" customHeight="1" r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" s="6" t="s">
         <v>69</v>
       </c>
@@ -1057,7 +1136,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row ht="30" customHeight="1" r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>5</v>
       </c>
@@ -1071,7 +1150,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row ht="30" customHeight="1" r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>8</v>
       </c>
@@ -1085,7 +1164,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row ht="30" customHeight="1" r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>10</v>
       </c>
@@ -1099,7 +1178,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row ht="30" customHeight="1" r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
         <v>12</v>
       </c>
@@ -1113,12 +1192,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row ht="30" customHeight="1" r="17" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C17" t="s">
-        <v>14</v>
+      <c r="C17" s="0" t="s">
+        <v>130</v>
       </c>
       <c r="D17" t="s">
         <v>101</v>
@@ -1127,7 +1206,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row ht="30" customHeight="1" r="18" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B18" s="6" t="s">
         <v>15</v>
       </c>
@@ -1141,367 +1220,255 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row ht="30" customHeight="1" r="19" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B19" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19" t="s">
-        <v>79</v>
+        <v>132</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="D19" s="0" t="s">
+        <v>142</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row ht="30" customHeight="1" r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" t="s">
-        <v>19</v>
-      </c>
-      <c r="D20" t="s">
-        <v>80</v>
+        <v>133</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="D20" s="0" t="s">
+        <v>143</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row ht="30" customHeight="1" r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C21" t="s">
-        <v>21</v>
-      </c>
-      <c r="D21" t="s">
-        <v>81</v>
+        <v>134</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="D21" s="0" t="s">
+        <v>146</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row ht="30" customHeight="1" r="22" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B22" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22" t="s">
-        <v>22</v>
-      </c>
-      <c r="D22" t="s">
-        <v>82</v>
+        <v>135</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="D22" s="0" t="s">
+        <v>145</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row ht="30" customHeight="1" r="23" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B23" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C23" t="s">
-        <v>24</v>
-      </c>
-      <c r="D23" t="s">
-        <v>83</v>
+        <v>136</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="D23" s="0" t="s">
+        <v>147</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row ht="30" customHeight="1" r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24" t="s">
-        <v>26</v>
-      </c>
-      <c r="D24" t="s">
-        <v>84</v>
+        <v>137</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="D24" s="0" t="s">
+        <v>141</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row ht="30" customHeight="1" r="25" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B25" s="6" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="C25" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="D25" t="s">
-        <v>85</v>
-      </c>
-      <c r="E25" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E25" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row ht="30" customHeight="1" r="26" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B26" s="6" t="s">
-        <v>29</v>
+        <v>103</v>
       </c>
       <c r="C26" t="s">
-        <v>30</v>
+        <v>103</v>
       </c>
       <c r="D26" t="s">
-        <v>86</v>
-      </c>
-      <c r="E26" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E26" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row ht="30" customHeight="1" r="27" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B27" s="6" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="C27" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="D27" t="s">
-        <v>87</v>
-      </c>
-      <c r="E27" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row ht="30" customHeight="1" r="28" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" t="s">
+        <v>51</v>
+      </c>
+      <c r="D28" t="s">
+        <v>95</v>
+      </c>
+      <c r="E28" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C28" t="s">
-        <v>34</v>
-      </c>
-      <c r="D28" t="s">
-        <v>88</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row ht="30" customHeight="1" r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" s="6" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="C29" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="D29" t="s">
-        <v>89</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row ht="30" customHeight="1" r="30" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B30" s="6" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="C30" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="D30" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="E30" s="7" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="31" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row ht="30" customHeight="1" r="31" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B31" s="6" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="C31" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="D31" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="32" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row ht="30" customHeight="1" r="32" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B32" s="6" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="C32" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="D32" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="33" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row ht="30" customHeight="1" r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" s="6" t="s">
-        <v>47</v>
+        <v>108</v>
       </c>
       <c r="C33" t="s">
-        <v>47</v>
+        <v>109</v>
       </c>
       <c r="D33" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row ht="30" customHeight="1" r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="6" t="s">
-        <v>103</v>
+        <v>60</v>
       </c>
       <c r="C34" t="s">
-        <v>103</v>
+        <v>61</v>
       </c>
       <c r="D34" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="35" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row ht="30" customHeight="1" r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" s="6" t="s">
-        <v>48</v>
+        <v>121</v>
       </c>
       <c r="C35" t="s">
-        <v>50</v>
+        <v>122</v>
       </c>
       <c r="D35" t="s">
-        <v>94</v>
+        <v>123</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="36" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row ht="30" customHeight="1" r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" s="6" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="C36" t="s">
-        <v>51</v>
+        <v>112</v>
       </c>
       <c r="D36" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="37" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C37" t="s">
-        <v>55</v>
-      </c>
-      <c r="D37" t="s">
-        <v>96</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C38" t="s">
-        <v>54</v>
-      </c>
-      <c r="D38" t="s">
-        <v>97</v>
-      </c>
-      <c r="E38" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="39" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C39" t="s">
-        <v>57</v>
-      </c>
-      <c r="D39" t="s">
-        <v>98</v>
-      </c>
-      <c r="E39" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="40" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C40" t="s">
-        <v>59</v>
-      </c>
-      <c r="D40" t="s">
-        <v>99</v>
-      </c>
-      <c r="E40" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="41" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="C41" t="s">
-        <v>109</v>
-      </c>
-      <c r="D41" t="s">
-        <v>110</v>
-      </c>
-      <c r="E41" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="42" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C42" t="s">
-        <v>61</v>
-      </c>
-      <c r="D42" t="s">
-        <v>100</v>
-      </c>
-      <c r="E42" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="43" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="C43" t="s">
-        <v>122</v>
-      </c>
-      <c r="D43" t="s">
-        <v>123</v>
-      </c>
-      <c r="E43" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="44" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C44" t="s">
-        <v>112</v>
-      </c>
-      <c r="D44" t="s">
-        <v>111</v>
-      </c>
-      <c r="E44" s="7" t="s">
         <v>64</v>
       </c>
     </row>

</xml_diff>